<commit_message>
ODE-1158 and ODE-1209 Addressed review comments. Also fixed another issue with bsmSource missing discovered during regression testing. Also added two more test case to the Test Report template.
</commit_message>
<xml_diff>
--- a/qa/ODE_TestReport_template.xlsx
+++ b/qa/ODE_TestReport_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\572682\ODTD\jpo-ode\qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CB20A8-A340-490D-9A91-C5AA528FBAEB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CD8206-FBAB-4AB7-9A0C-D0B037A5B729}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8363" windowWidth="25598" windowHeight="15540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="8363" windowWidth="25598" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BSM" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="77">
   <si>
     <t>Data Element</t>
   </si>
@@ -282,20 +282,23 @@
     <t>All records within a file comply with the following rules:</t>
   </si>
   <si>
-    <t>metadata.serialId.recordId is mostly sequencial and void of huge gaps or duplication</t>
-  </si>
-  <si>
-    <t>metadata.serialId.serialNumber is mostly sequencial and void of huge gaps or duplication</t>
-  </si>
-  <si>
-    <t>metadata.serialId.recordGeneratedAt is mostly chronological and void of huge gaps or duplication</t>
-  </si>
-  <si>
-    <t>metadata.serialId.odeReceivedAt is mostly sequencial and void of huge gaps or duplication</t>
-  </si>
-  <si>
     <t>Required, Optional, Absent
 (R | O | A)</t>
+  </si>
+  <si>
+    <t>metadata.serialId.bundleSize is EQUAL TO number of output JSON records</t>
+  </si>
+  <si>
+    <t>metadata.serialId.serialNumber is mostly sequencial and void of ANY gaps or duplication</t>
+  </si>
+  <si>
+    <t>metadata.serialId.recordId is mostly sequencial and void of ANY gaps or duplication</t>
+  </si>
+  <si>
+    <t>metadata.serialId.recordGeneratedAt is mostly chronological and void of any HUGE gaps or duplication</t>
+  </si>
+  <si>
+    <t>metadata.serialId.odeReceivedAt is mostly sequencial and void of any HUGE gaps or duplication</t>
   </si>
 </sst>
 </file>
@@ -352,7 +355,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -424,24 +427,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -488,9 +478,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -507,7 +494,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="59">
+  <dxfs count="38">
     <dxf>
       <font>
         <color rgb="FF00B050"/>
@@ -570,31 +557,21 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFFFFF00"/>
+        <color rgb="FF00B050"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFFFFF00"/>
+        <color rgb="FFFF0000"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -620,11 +597,41 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFFFFF00"/>
+        <color rgb="FF00B050"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -660,251 +667,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -935,6 +697,21 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
         <right style="medium">
           <color indexed="64"/>
         </right>
@@ -1040,45 +817,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C7CB36D7-5FCC-4F93-8C5C-DB1AD33CEE26}" name="Table1" displayName="Table1" ref="A1:G1048571" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
-  <autoFilter ref="A1:G1048571" xr:uid="{0930BACC-7465-4555-B7D0-81DB76F717E2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C7CB36D7-5FCC-4F93-8C5C-DB1AD33CEE26}" name="Table1" displayName="Table1" ref="A1:G1048572" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+  <autoFilter ref="A1:G1048572" xr:uid="{0930BACC-7465-4555-B7D0-81DB76F717E2}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{47C74D4F-C384-41D6-AC9A-66ABA3FB7E8F}" name="Data Element" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{99B4F80A-89ED-40D3-9D45-69CA8ECFDB94}" name="Data Element Type_x000a_(string, enum, number)" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{CAAE2223-B9F2-485D-9CB7-A4AAF2BBC93E}" name="Valid Range" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{86A478FB-AF4B-4492-AFD0-43D824D3FC51}" name="Required, Optional, Absent_x000a_(R | O | A)" dataDxfId="53"/>
-    <tableColumn id="5" xr3:uid="{B015FFC9-4721-49D8-85F6-76E354562271}" name="bsmLogDuringEvent Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="52"/>
-    <tableColumn id="7" xr3:uid="{D33782C4-7B1B-42DD-A19C-AEA42EADF11E}" name="bsmTx Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="51"/>
-    <tableColumn id="13" xr3:uid="{8E33C4D1-AA5C-49F7-A10C-0B61296C591B}" name="rxMsg_BSM Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{47C74D4F-C384-41D6-AC9A-66ABA3FB7E8F}" name="Data Element" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{99B4F80A-89ED-40D3-9D45-69CA8ECFDB94}" name="Data Element Type_x000a_(string, enum, number)" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{CAAE2223-B9F2-485D-9CB7-A4AAF2BBC93E}" name="Valid Range" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{86A478FB-AF4B-4492-AFD0-43D824D3FC51}" name="Required, Optional, Absent_x000a_(R | O | A)" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{B015FFC9-4721-49D8-85F6-76E354562271}" name="bsmLogDuringEvent Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{D33782C4-7B1B-42DD-A19C-AEA42EADF11E}" name="bsmTx Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="30"/>
+    <tableColumn id="13" xr3:uid="{8E33C4D1-AA5C-49F7-A10C-0B61296C591B}" name="rxMsg_BSM Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F042E017-DBDF-4B1A-AAA4-37B2FE011BAA}" name="Table13" displayName="Table13" ref="A1:F1048576" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F042E017-DBDF-4B1A-AAA4-37B2FE011BAA}" name="Table13" displayName="Table13" ref="A1:F1048576" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A1:F1048576" xr:uid="{0930BACC-7465-4555-B7D0-81DB76F717E2}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{3F33CB0F-F50B-4B03-8252-01463C6C7074}" name="Data Element" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{BE6E9B1B-CCCB-4CA6-AF50-F3F53905D733}" name="Data Element Type_x000a_(string, enum, number)" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{80732682-D436-4CA8-85C0-C71E4C3EB979}" name="Valid Range" dataDxfId="45"/>
-    <tableColumn id="8" xr3:uid="{09C1C98D-CC2F-48C6-8DF2-F8A850937D6E}" name="Required, Optional, Absent_x000a_(R | O | A)" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{36FF3B94-1467-475C-B2D1-7AF20DAA39C6}" name="dnMsg Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="44"/>
-    <tableColumn id="15" xr3:uid="{EF8CFFBA-3DF5-4F38-A44E-D0335644E9F9}" name="rxMsg_TIM Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="43"/>
+    <tableColumn id="1" xr3:uid="{3F33CB0F-F50B-4B03-8252-01463C6C7074}" name="Data Element" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{BE6E9B1B-CCCB-4CA6-AF50-F3F53905D733}" name="Data Element Type_x000a_(string, enum, number)" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{80732682-D436-4CA8-85C0-C71E4C3EB979}" name="Valid Range" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{09C1C98D-CC2F-48C6-8DF2-F8A850937D6E}" name="Required, Optional, Absent_x000a_(R | O | A)" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{36FF3B94-1467-475C-B2D1-7AF20DAA39C6}" name="dnMsg Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="22"/>
+    <tableColumn id="15" xr3:uid="{EF8CFFBA-3DF5-4F38-A44E-D0335644E9F9}" name="rxMsg_TIM Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5BD2B0BF-B871-477D-ABCF-5BC75EDEB989}" name="Table134" displayName="Table134" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5BD2B0BF-B871-477D-ABCF-5BC75EDEB989}" name="Table134" displayName="Table134" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:E1048576" xr:uid="{0930BACC-7465-4555-B7D0-81DB76F717E2}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F0DCAC9D-56A6-4611-9A8B-21A45430DA1F}" name="Data Element" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{31562A37-A54A-4B17-846B-9919E28099EB}" name="Data Element Type_x000a_(string, enum, number)" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{848A6CED-2D39-48D6-A8E3-69F28177AF62}" name="Valid Range" dataDxfId="38"/>
-    <tableColumn id="10" xr3:uid="{0F25FFC7-417F-4EFA-AA0F-49E26202A0AF}" name="Required, Optional, Absent_x000a_(R | O | A)" dataDxfId="13"/>
-    <tableColumn id="11" xr3:uid="{9A376F7F-22DD-4BC0-BBDF-61339AE77B5D}" name="driverAlert Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{F0DCAC9D-56A6-4611-9A8B-21A45430DA1F}" name="Data Element" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{31562A37-A54A-4B17-846B-9919E28099EB}" name="Data Element Type_x000a_(string, enum, number)" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{848A6CED-2D39-48D6-A8E3-69F28177AF62}" name="Valid Range" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{0F25FFC7-417F-4EFA-AA0F-49E26202A0AF}" name="Required, Optional, Absent_x000a_(R | O | A)" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{9A376F7F-22DD-4BC0-BBDF-61339AE77B5D}" name="driverAlert Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1347,11 +1124,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1:K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1376,7 +1153,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
@@ -1387,12 +1164,12 @@
       <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A2" s="7" t="s">
@@ -1890,12 +1667,12 @@
       <c r="G33" s="14"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A34" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="9" t="s">
+      <c r="A34" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="15" t="s">
         <v>19</v>
       </c>
       <c r="E34" s="14"/>
@@ -1903,12 +1680,12 @@
       <c r="G34" s="14"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A35" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="9" t="s">
+      <c r="A35" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="15" t="s">
         <v>19</v>
       </c>
       <c r="E35" s="14"/>
@@ -1916,12 +1693,12 @@
       <c r="G35" s="14"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A36" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="9" t="s">
+      <c r="A36" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="15" t="s">
         <v>19</v>
       </c>
       <c r="E36" s="14"/>
@@ -1929,12 +1706,12 @@
       <c r="G36" s="14"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A37" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="9" t="s">
+      <c r="A37" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="15" t="s">
         <v>19</v>
       </c>
       <c r="E37" s="14"/>
@@ -1942,24 +1719,26 @@
       <c r="G37" s="14"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A38" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="15" t="s">
+        <v>19</v>
+      </c>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
       <c r="G38" s="14"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A39" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="9"/>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
       <c r="G39" s="14"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A40" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -1969,7 +1748,9 @@
       <c r="G40" s="14"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A41" s="7"/>
+      <c r="A41" s="7" t="s">
+        <v>65</v>
+      </c>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="9"/>
@@ -1986,18 +1767,37 @@
       <c r="F42" s="14"/>
       <c r="G42" s="14"/>
     </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="H1:K1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E2:G42">
-    <cfRule type="expression" dxfId="1" priority="2">
+  <conditionalFormatting sqref="E2:G33 E39:G43 F34:G38">
+    <cfRule type="expression" dxfId="13" priority="4">
       <formula>AND(NOT(ISBLANK(E2)),OR(AND($D2="R",E2&lt;&gt;"V"),AND($D2="A",E2&lt;&gt;"M")))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:G42">
+  <conditionalFormatting sqref="E2:G33 E39:G43 F34:G38">
+    <cfRule type="expression" dxfId="12" priority="3">
+      <formula>AND(NOT(ISBLANK(E2)),OR(AND($D2="R",E2="V"),AND($D2="R",E2="v")))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34:E38">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>AND(NOT(ISBLANK(E34)),OR(AND($D34="R",E34&lt;&gt;"V"),AND($D34="A",E34&lt;&gt;"M")))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34:E38">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND(NOT(ISBLANK(E2)),OR(AND($D2="R",E2="V"),AND($D2="R",E2="v")))</formula>
+      <formula>AND(NOT(ISBLANK(E34)),OR(AND($D34="R",E34="V"),AND($D34="R",E34="v")))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2010,11 +1810,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63391549-4B32-4952-900C-D9235D0C5642}">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1:J1"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34:E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -2038,8 +1838,8 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>75</v>
+      <c r="D1" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>4</v>
@@ -2047,12 +1847,12 @@
       <c r="F1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A2" s="7" t="s">
@@ -2519,7 +2319,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A34" s="10" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
@@ -2531,7 +2331,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A35" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
@@ -2543,7 +2343,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A36" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
@@ -2553,30 +2353,51 @@
       <c r="E36" s="14"/>
       <c r="F36" s="14"/>
     </row>
-    <row r="37" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A37" s="10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
-      <c r="D37" s="16" t="s">
+      <c r="D37" s="15" t="s">
         <v>19</v>
       </c>
       <c r="E37" s="14"/>
       <c r="F37" s="14"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A38" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="G1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E2:F37">
-    <cfRule type="expression" dxfId="3" priority="2">
+  <conditionalFormatting sqref="E2:F33 F34:F37">
+    <cfRule type="expression" dxfId="11" priority="4">
       <formula>AND(NOT(ISBLANK(E2)),OR(AND($D2="R",E2&lt;&gt;"V"),AND($D2="A",E2&lt;&gt;"M")))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:F37">
-    <cfRule type="expression" dxfId="2" priority="1">
+  <conditionalFormatting sqref="E2:F33 F34:F37">
+    <cfRule type="expression" dxfId="10" priority="3">
       <formula>AND(NOT(ISBLANK(E2)),OR(AND($D2="R",E2="V"),AND($D2="R",E2="v")))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34:E38">
+    <cfRule type="expression" dxfId="9" priority="2">
+      <formula>AND(NOT(ISBLANK(E34)),OR(AND($D34="R",E34&lt;&gt;"V"),AND($D34="A",E34&lt;&gt;"M")))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34:E38">
+    <cfRule type="expression" dxfId="8" priority="1">
+      <formula>AND(NOT(ISBLANK(E34)),OR(AND($D34="R",E34="V"),AND($D34="R",E34="v")))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2589,11 +2410,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1C3D962-EA84-4A6E-9926-C561BC5A7D51}">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36:E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -2616,18 +2437,18 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="17" t="s">
+      <c r="D1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" s="7" t="s">
@@ -2639,7 +2460,7 @@
       <c r="C2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="17" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3046,7 +2867,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A36" s="10" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
@@ -3056,7 +2877,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A37" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
@@ -3066,7 +2887,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A38" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
@@ -3074,13 +2895,23 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A39" s="10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
-      <c r="D39" s="16" t="s">
+      <c r="D39" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A40" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="15" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3089,22 +2920,22 @@
     <mergeCell ref="F1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="E2">
-    <cfRule type="expression" dxfId="10" priority="5">
+    <cfRule type="expression" dxfId="7" priority="7">
       <formula>AND(NOT(ISBLANK(E2)),OR(AND($D2="R",E2&lt;&gt;"V"),AND($D2="A",E2&lt;&gt;"M")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>AND(NOT(ISBLANK(E2)),OR(AND($D2="R",E2="V"),AND($D2="R",E2="v")))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E39">
-    <cfRule type="expression" dxfId="5" priority="2">
+  <conditionalFormatting sqref="E3:E40">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>AND(NOT(ISBLANK(E3)),OR(AND($D3="R",E3&lt;&gt;"V"),AND($D3="A",E3&lt;&gt;"M")))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E39">
-    <cfRule type="expression" dxfId="4" priority="1">
+  <conditionalFormatting sqref="E3:E40">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>AND(NOT(ISBLANK(E3)),OR(AND($D3="R",E3="V"),AND($D3="R",E3="v")))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
ODE-1206 COrrected bsmSource as A (Absent) for non-BSM records.
</commit_message>
<xml_diff>
--- a/qa/ODE_TestReport_template.xlsx
+++ b/qa/ODE_TestReport_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\572682\ODTD\jpo-ode\qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CD8206-FBAB-4AB7-9A0C-D0B037A5B729}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD25420-BCE4-4F5D-834D-5CECD5C90B76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8363" windowWidth="25598" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="8363" windowWidth="25598" windowHeight="15540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BSM" sheetId="1" r:id="rId1"/>
@@ -494,147 +494,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="36">
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -681,6 +541,46 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -737,6 +637,46 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -802,6 +742,46 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -817,45 +797,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C7CB36D7-5FCC-4F93-8C5C-DB1AD33CEE26}" name="Table1" displayName="Table1" ref="A1:G1048572" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C7CB36D7-5FCC-4F93-8C5C-DB1AD33CEE26}" name="Table1" displayName="Table1" ref="A1:G1048572" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A1:G1048572" xr:uid="{0930BACC-7465-4555-B7D0-81DB76F717E2}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{47C74D4F-C384-41D6-AC9A-66ABA3FB7E8F}" name="Data Element" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{99B4F80A-89ED-40D3-9D45-69CA8ECFDB94}" name="Data Element Type_x000a_(string, enum, number)" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{CAAE2223-B9F2-485D-9CB7-A4AAF2BBC93E}" name="Valid Range" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{86A478FB-AF4B-4492-AFD0-43D824D3FC51}" name="Required, Optional, Absent_x000a_(R | O | A)" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{B015FFC9-4721-49D8-85F6-76E354562271}" name="bsmLogDuringEvent Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{D33782C4-7B1B-42DD-A19C-AEA42EADF11E}" name="bsmTx Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="30"/>
-    <tableColumn id="13" xr3:uid="{8E33C4D1-AA5C-49F7-A10C-0B61296C591B}" name="rxMsg_BSM Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{47C74D4F-C384-41D6-AC9A-66ABA3FB7E8F}" name="Data Element" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{99B4F80A-89ED-40D3-9D45-69CA8ECFDB94}" name="Data Element Type_x000a_(string, enum, number)" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{CAAE2223-B9F2-485D-9CB7-A4AAF2BBC93E}" name="Valid Range" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{86A478FB-AF4B-4492-AFD0-43D824D3FC51}" name="Required, Optional, Absent_x000a_(R | O | A)" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{B015FFC9-4721-49D8-85F6-76E354562271}" name="bsmLogDuringEvent Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{D33782C4-7B1B-42DD-A19C-AEA42EADF11E}" name="bsmTx Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="24"/>
+    <tableColumn id="13" xr3:uid="{8E33C4D1-AA5C-49F7-A10C-0B61296C591B}" name="rxMsg_BSM Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F042E017-DBDF-4B1A-AAA4-37B2FE011BAA}" name="Table13" displayName="Table13" ref="A1:F1048576" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F042E017-DBDF-4B1A-AAA4-37B2FE011BAA}" name="Table13" displayName="Table13" ref="A1:F1048576" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A1:F1048576" xr:uid="{0930BACC-7465-4555-B7D0-81DB76F717E2}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{3F33CB0F-F50B-4B03-8252-01463C6C7074}" name="Data Element" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{BE6E9B1B-CCCB-4CA6-AF50-F3F53905D733}" name="Data Element Type_x000a_(string, enum, number)" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{80732682-D436-4CA8-85C0-C71E4C3EB979}" name="Valid Range" dataDxfId="24"/>
-    <tableColumn id="8" xr3:uid="{09C1C98D-CC2F-48C6-8DF2-F8A850937D6E}" name="Required, Optional, Absent_x000a_(R | O | A)" dataDxfId="23"/>
-    <tableColumn id="9" xr3:uid="{36FF3B94-1467-475C-B2D1-7AF20DAA39C6}" name="dnMsg Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="22"/>
-    <tableColumn id="15" xr3:uid="{EF8CFFBA-3DF5-4F38-A44E-D0335644E9F9}" name="rxMsg_TIM Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{3F33CB0F-F50B-4B03-8252-01463C6C7074}" name="Data Element" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{BE6E9B1B-CCCB-4CA6-AF50-F3F53905D733}" name="Data Element Type_x000a_(string, enum, number)" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{80732682-D436-4CA8-85C0-C71E4C3EB979}" name="Valid Range" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{09C1C98D-CC2F-48C6-8DF2-F8A850937D6E}" name="Required, Optional, Absent_x000a_(R | O | A)" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{36FF3B94-1467-475C-B2D1-7AF20DAA39C6}" name="dnMsg Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="12"/>
+    <tableColumn id="15" xr3:uid="{EF8CFFBA-3DF5-4F38-A44E-D0335644E9F9}" name="rxMsg_TIM Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5BD2B0BF-B871-477D-ABCF-5BC75EDEB989}" name="Table134" displayName="Table134" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5BD2B0BF-B871-477D-ABCF-5BC75EDEB989}" name="Table134" displayName="Table134" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E1048576" xr:uid="{0930BACC-7465-4555-B7D0-81DB76F717E2}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F0DCAC9D-56A6-4611-9A8B-21A45430DA1F}" name="Data Element" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{31562A37-A54A-4B17-846B-9919E28099EB}" name="Data Element Type_x000a_(string, enum, number)" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{848A6CED-2D39-48D6-A8E3-69F28177AF62}" name="Valid Range" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{0F25FFC7-417F-4EFA-AA0F-49E26202A0AF}" name="Required, Optional, Absent_x000a_(R | O | A)" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{9A376F7F-22DD-4BC0-BBDF-61339AE77B5D}" name="driverAlert Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{F0DCAC9D-56A6-4611-9A8B-21A45430DA1F}" name="Data Element" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{31562A37-A54A-4B17-846B-9919E28099EB}" name="Data Element Type_x000a_(string, enum, number)" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{848A6CED-2D39-48D6-A8E3-69F28177AF62}" name="Valid Range" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{0F25FFC7-417F-4EFA-AA0F-49E26202A0AF}" name="Required, Optional, Absent_x000a_(R | O | A)" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{9A376F7F-22DD-4BC0-BBDF-61339AE77B5D}" name="driverAlert Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1126,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
@@ -1781,22 +1761,22 @@
     <mergeCell ref="H1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="E2:G33 E39:G43 F34:G38">
-    <cfRule type="expression" dxfId="13" priority="4">
+    <cfRule type="expression" dxfId="35" priority="4">
       <formula>AND(NOT(ISBLANK(E2)),OR(AND($D2="R",E2&lt;&gt;"V"),AND($D2="A",E2&lt;&gt;"M")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:G33 E39:G43 F34:G38">
-    <cfRule type="expression" dxfId="12" priority="3">
+    <cfRule type="expression" dxfId="34" priority="3">
       <formula>AND(NOT(ISBLANK(E2)),OR(AND($D2="R",E2="V"),AND($D2="R",E2="v")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34:E38">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="33" priority="2">
       <formula>AND(NOT(ISBLANK(E34)),OR(AND($D34="R",E34&lt;&gt;"V"),AND($D34="A",E34&lt;&gt;"M")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34:E38">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="32" priority="1">
       <formula>AND(NOT(ISBLANK(E34)),OR(AND($D34="R",E34="V"),AND($D34="R",E34="v")))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1813,8 +1793,8 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34:E38"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1865,7 +1845,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
@@ -2381,22 +2361,22 @@
     <mergeCell ref="G1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="E2:F33 F34:F37">
-    <cfRule type="expression" dxfId="11" priority="4">
+    <cfRule type="expression" dxfId="22" priority="4">
       <formula>AND(NOT(ISBLANK(E2)),OR(AND($D2="R",E2&lt;&gt;"V"),AND($D2="A",E2&lt;&gt;"M")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:F33 F34:F37">
-    <cfRule type="expression" dxfId="10" priority="3">
+    <cfRule type="expression" dxfId="21" priority="3">
       <formula>AND(NOT(ISBLANK(E2)),OR(AND($D2="R",E2="V"),AND($D2="R",E2="v")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34:E38">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="20" priority="2">
       <formula>AND(NOT(ISBLANK(E34)),OR(AND($D34="R",E34&lt;&gt;"V"),AND($D34="A",E34&lt;&gt;"M")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34:E38">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="19" priority="1">
       <formula>AND(NOT(ISBLANK(E34)),OR(AND($D34="R",E34="V"),AND($D34="R",E34="v")))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2412,9 +2392,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1C3D962-EA84-4A6E-9926-C561BC5A7D51}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A36" sqref="A36:E40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -2461,7 +2441,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.5">
@@ -2920,22 +2900,22 @@
     <mergeCell ref="F1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="E2">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="10" priority="7">
       <formula>AND(NOT(ISBLANK(E2)),OR(AND($D2="R",E2&lt;&gt;"V"),AND($D2="A",E2&lt;&gt;"M")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>AND(NOT(ISBLANK(E2)),OR(AND($D2="R",E2="V"),AND($D2="R",E2="v")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E40">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>AND(NOT(ISBLANK(E3)),OR(AND($D3="R",E3&lt;&gt;"V"),AND($D3="A",E3&lt;&gt;"M")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E40">
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>AND(NOT(ISBLANK(E3)),OR(AND($D3="R",E3="V"),AND($D3="R",E3="v")))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
ODE-1206 added TIM Broadcast page to Test Reports template.
</commit_message>
<xml_diff>
--- a/qa/ODE_TestReport_template.xlsx
+++ b/qa/ODE_TestReport_template.xlsx
@@ -8,43 +8,53 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\572682\ODTD\jpo-ode\qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD25420-BCE4-4F5D-834D-5CECD5C90B76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD12CA3-D01F-4571-B263-AE2FE283BEDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8363" windowWidth="25598" windowHeight="15540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="8363" windowWidth="25598" windowHeight="15540" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BSM" sheetId="1" r:id="rId1"/>
     <sheet name="TIM" sheetId="2" r:id="rId2"/>
     <sheet name="Driver Alert" sheetId="3" r:id="rId3"/>
+    <sheet name="TIM Broadcast" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_edn1" localSheetId="0">BSM!$A$28</definedName>
     <definedName name="_edn1" localSheetId="2">'Driver Alert'!$A$28</definedName>
     <definedName name="_edn1" localSheetId="1">TIM!$A$28</definedName>
+    <definedName name="_edn1" localSheetId="3">'TIM Broadcast'!$A$28</definedName>
     <definedName name="_ftn1" localSheetId="0">BSM!$A$22</definedName>
     <definedName name="_ftn1" localSheetId="2">'Driver Alert'!$A$22</definedName>
     <definedName name="_ftn1" localSheetId="1">TIM!$A$22</definedName>
+    <definedName name="_ftn1" localSheetId="3">'TIM Broadcast'!$A$22</definedName>
     <definedName name="_ftn2" localSheetId="0">BSM!$A$23</definedName>
     <definedName name="_ftn2" localSheetId="2">'Driver Alert'!$A$23</definedName>
     <definedName name="_ftn2" localSheetId="1">TIM!$A$23</definedName>
+    <definedName name="_ftn2" localSheetId="3">'TIM Broadcast'!$A$23</definedName>
     <definedName name="_ftn3" localSheetId="0">BSM!$A$24</definedName>
     <definedName name="_ftn3" localSheetId="2">'Driver Alert'!$A$24</definedName>
     <definedName name="_ftn3" localSheetId="1">TIM!$A$24</definedName>
+    <definedName name="_ftn3" localSheetId="3">'TIM Broadcast'!$A$24</definedName>
     <definedName name="_ftn4" localSheetId="0">BSM!$A$25</definedName>
     <definedName name="_ftn4" localSheetId="2">'Driver Alert'!$A$25</definedName>
     <definedName name="_ftn4" localSheetId="1">TIM!$A$25</definedName>
+    <definedName name="_ftn4" localSheetId="3">'TIM Broadcast'!$A$25</definedName>
     <definedName name="_ftnref1" localSheetId="0">BSM!$A$2</definedName>
     <definedName name="_ftnref1" localSheetId="2">'Driver Alert'!$A$2</definedName>
     <definedName name="_ftnref1" localSheetId="1">TIM!$A$2</definedName>
+    <definedName name="_ftnref1" localSheetId="3">'TIM Broadcast'!$A$2</definedName>
     <definedName name="_ftnref3" localSheetId="0">BSM!$A$10</definedName>
     <definedName name="_ftnref3" localSheetId="2">'Driver Alert'!$A$10</definedName>
     <definedName name="_ftnref3" localSheetId="1">TIM!$A$10</definedName>
+    <definedName name="_ftnref3" localSheetId="3">'TIM Broadcast'!$A$10</definedName>
     <definedName name="_ftnref4" localSheetId="0">BSM!$A$18</definedName>
     <definedName name="_ftnref4" localSheetId="2">'Driver Alert'!$A$18</definedName>
     <definedName name="_ftnref4" localSheetId="1">TIM!$A$18</definedName>
+    <definedName name="_ftnref4" localSheetId="3">'TIM Broadcast'!$A$18</definedName>
     <definedName name="_Ref512500396" localSheetId="0">BSM!$A$18</definedName>
     <definedName name="_Ref512500396" localSheetId="2">'Driver Alert'!$A$18</definedName>
     <definedName name="_Ref512500396" localSheetId="1">TIM!$A$18</definedName>
+    <definedName name="_Ref512500396" localSheetId="3">'TIM Broadcast'!$A$18</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -64,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="117">
   <si>
     <t>Data Element</t>
   </si>
@@ -299,6 +309,126 @@
   </si>
   <si>
     <t>metadata.serialId.odeReceivedAt is mostly sequencial and void of any HUGE gaps or duplication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "request": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "ode": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "verb": "POST",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "version": 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "sdw": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "serviceRegion": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          "nwCorner": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "latitude": 44.998459,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "longitude": -111.040817</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          "seCorner": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "latitude": 41.104674,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "longitude": -104.111312</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "ttl": "oneweek"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "rsus": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "rsus": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          "rsuTarget": "127.0.0.3",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          "rsuUsername": "v3user",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          "rsuRetries": 1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          "rsuTimeout": 1000,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          "rsuPassword": "*",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          "rsuIndex": 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "snmp": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "mode": 1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "deliverystop": "2018-01-01T17:47:11-05:15",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "rsuid": "00000083",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "deliverystart": "2017-06-01T17:47:11-05:00",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "enable": 1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "channel": 178,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "msgid": 31,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "interval": 2,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "status": 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    },</t>
+  </si>
+  <si>
+    <t>TravelerInformation Present and Valid, Present and Invalid, Missing (V, I, M)</t>
+  </si>
+  <si>
+    <t>OdeTravelerInformationMessage Present and Valid, Present and Invalid, Missing (V, I, M)2</t>
   </si>
 </sst>
 </file>
@@ -494,7 +624,213 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="50">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -512,18 +848,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -535,63 +859,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -623,6 +891,18 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -634,47 +914,10 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -692,7 +935,9 @@
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
         <right style="medium">
           <color indexed="64"/>
         </right>
@@ -701,6 +946,21 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -718,6 +978,32 @@
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -742,46 +1028,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -797,45 +1043,60 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C7CB36D7-5FCC-4F93-8C5C-DB1AD33CEE26}" name="Table1" displayName="Table1" ref="A1:G1048572" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C7CB36D7-5FCC-4F93-8C5C-DB1AD33CEE26}" name="Table1" displayName="Table1" ref="A1:G1048572" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
   <autoFilter ref="A1:G1048572" xr:uid="{0930BACC-7465-4555-B7D0-81DB76F717E2}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{47C74D4F-C384-41D6-AC9A-66ABA3FB7E8F}" name="Data Element" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{99B4F80A-89ED-40D3-9D45-69CA8ECFDB94}" name="Data Element Type_x000a_(string, enum, number)" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{CAAE2223-B9F2-485D-9CB7-A4AAF2BBC93E}" name="Valid Range" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{86A478FB-AF4B-4492-AFD0-43D824D3FC51}" name="Required, Optional, Absent_x000a_(R | O | A)" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{B015FFC9-4721-49D8-85F6-76E354562271}" name="bsmLogDuringEvent Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{D33782C4-7B1B-42DD-A19C-AEA42EADF11E}" name="bsmTx Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="24"/>
-    <tableColumn id="13" xr3:uid="{8E33C4D1-AA5C-49F7-A10C-0B61296C591B}" name="rxMsg_BSM Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{47C74D4F-C384-41D6-AC9A-66ABA3FB7E8F}" name="Data Element" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{99B4F80A-89ED-40D3-9D45-69CA8ECFDB94}" name="Data Element Type_x000a_(string, enum, number)" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{CAAE2223-B9F2-485D-9CB7-A4AAF2BBC93E}" name="Valid Range" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{86A478FB-AF4B-4492-AFD0-43D824D3FC51}" name="Required, Optional, Absent_x000a_(R | O | A)" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{B015FFC9-4721-49D8-85F6-76E354562271}" name="bsmLogDuringEvent Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="43"/>
+    <tableColumn id="7" xr3:uid="{D33782C4-7B1B-42DD-A19C-AEA42EADF11E}" name="bsmTx Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="42"/>
+    <tableColumn id="13" xr3:uid="{8E33C4D1-AA5C-49F7-A10C-0B61296C591B}" name="rxMsg_BSM Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F042E017-DBDF-4B1A-AAA4-37B2FE011BAA}" name="Table13" displayName="Table13" ref="A1:F1048576" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F042E017-DBDF-4B1A-AAA4-37B2FE011BAA}" name="Table13" displayName="Table13" ref="A1:F1048576" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <autoFilter ref="A1:F1048576" xr:uid="{0930BACC-7465-4555-B7D0-81DB76F717E2}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{3F33CB0F-F50B-4B03-8252-01463C6C7074}" name="Data Element" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{BE6E9B1B-CCCB-4CA6-AF50-F3F53905D733}" name="Data Element Type_x000a_(string, enum, number)" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{80732682-D436-4CA8-85C0-C71E4C3EB979}" name="Valid Range" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{09C1C98D-CC2F-48C6-8DF2-F8A850937D6E}" name="Required, Optional, Absent_x000a_(R | O | A)" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{36FF3B94-1467-475C-B2D1-7AF20DAA39C6}" name="dnMsg Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="12"/>
-    <tableColumn id="15" xr3:uid="{EF8CFFBA-3DF5-4F38-A44E-D0335644E9F9}" name="rxMsg_TIM Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{3F33CB0F-F50B-4B03-8252-01463C6C7074}" name="Data Element" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{BE6E9B1B-CCCB-4CA6-AF50-F3F53905D733}" name="Data Element Type_x000a_(string, enum, number)" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{80732682-D436-4CA8-85C0-C71E4C3EB979}" name="Valid Range" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{09C1C98D-CC2F-48C6-8DF2-F8A850937D6E}" name="Required, Optional, Absent_x000a_(R | O | A)" dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{36FF3B94-1467-475C-B2D1-7AF20DAA39C6}" name="dnMsg Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{58EB541E-74D9-4581-AC24-0B872CC49439}" name="rxMsg_TIM Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5BD2B0BF-B871-477D-ABCF-5BC75EDEB989}" name="Table134" displayName="Table134" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5BD2B0BF-B871-477D-ABCF-5BC75EDEB989}" name="Table134" displayName="Table134" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="A1:E1048576" xr:uid="{0930BACC-7465-4555-B7D0-81DB76F717E2}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F0DCAC9D-56A6-4611-9A8B-21A45430DA1F}" name="Data Element" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{31562A37-A54A-4B17-846B-9919E28099EB}" name="Data Element Type_x000a_(string, enum, number)" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{848A6CED-2D39-48D6-A8E3-69F28177AF62}" name="Valid Range" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{0F25FFC7-417F-4EFA-AA0F-49E26202A0AF}" name="Required, Optional, Absent_x000a_(R | O | A)" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{9A376F7F-22DD-4BC0-BBDF-61339AE77B5D}" name="driverAlert Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{F0DCAC9D-56A6-4611-9A8B-21A45430DA1F}" name="Data Element" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{31562A37-A54A-4B17-846B-9919E28099EB}" name="Data Element Type_x000a_(string, enum, number)" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{848A6CED-2D39-48D6-A8E3-69F28177AF62}" name="Valid Range" dataDxfId="29"/>
+    <tableColumn id="10" xr3:uid="{0F25FFC7-417F-4EFA-AA0F-49E26202A0AF}" name="Required, Optional, Absent_x000a_(R | O | A)" dataDxfId="28"/>
+    <tableColumn id="11" xr3:uid="{9A376F7F-22DD-4BC0-BBDF-61339AE77B5D}" name="driverAlert Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="27"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DA290B07-4F49-4E32-BA1D-3D7E04A03CA3}" name="Table135" displayName="Table135" ref="A1:F1048576" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="A1:F1048576" xr:uid="{0930BACC-7465-4555-B7D0-81DB76F717E2}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{7BDA7C9B-5F07-447F-9932-BCFA2C4986EC}" name="Data Element" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{3A98A276-5EA3-41B1-8EDB-5CD7686A7190}" name="Data Element Type_x000a_(string, enum, number)" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{D9E0A608-B786-49B1-AA76-974FA2D657E3}" name="Valid Range" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{CB80B222-D637-4313-BD7A-0DA5B2FF5A07}" name="Required, Optional, Absent_x000a_(R | O | A)" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{431B1286-E99D-419A-A24E-B230FAB1C9EB}" name="TravelerInformation Present and Valid, Present and Invalid, Missing (V, I, M)" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{4D01B887-8E3B-414F-859B-2C86ABC27762}" name="OdeTravelerInformationMessage Present and Valid, Present and Invalid, Missing (V, I, M)2" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1761,22 +2022,22 @@
     <mergeCell ref="H1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="E2:G33 E39:G43 F34:G38">
-    <cfRule type="expression" dxfId="35" priority="4">
+    <cfRule type="expression" dxfId="18" priority="4">
       <formula>AND(NOT(ISBLANK(E2)),OR(AND($D2="R",E2&lt;&gt;"V"),AND($D2="A",E2&lt;&gt;"M")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:G33 E39:G43 F34:G38">
-    <cfRule type="expression" dxfId="34" priority="3">
+    <cfRule type="expression" dxfId="17" priority="3">
       <formula>AND(NOT(ISBLANK(E2)),OR(AND($D2="R",E2="V"),AND($D2="R",E2="v")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34:E38">
-    <cfRule type="expression" dxfId="33" priority="2">
+    <cfRule type="expression" dxfId="16" priority="2">
       <formula>AND(NOT(ISBLANK(E34)),OR(AND($D34="R",E34&lt;&gt;"V"),AND($D34="A",E34&lt;&gt;"M")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34:E38">
-    <cfRule type="expression" dxfId="32" priority="1">
+    <cfRule type="expression" dxfId="15" priority="1">
       <formula>AND(NOT(ISBLANK(E34)),OR(AND($D34="R",E34="V"),AND($D34="R",E34="v")))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1794,7 +2055,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -2360,24 +2621,34 @@
   <mergeCells count="1">
     <mergeCell ref="G1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E2:F33 F34:F37">
-    <cfRule type="expression" dxfId="22" priority="4">
+  <conditionalFormatting sqref="E2:E33">
+    <cfRule type="expression" dxfId="14" priority="8">
       <formula>AND(NOT(ISBLANK(E2)),OR(AND($D2="R",E2&lt;&gt;"V"),AND($D2="A",E2&lt;&gt;"M")))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:F33 F34:F37">
-    <cfRule type="expression" dxfId="21" priority="3">
+  <conditionalFormatting sqref="E2:E33">
+    <cfRule type="expression" dxfId="13" priority="7">
       <formula>AND(NOT(ISBLANK(E2)),OR(AND($D2="R",E2="V"),AND($D2="R",E2="v")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34:E38">
-    <cfRule type="expression" dxfId="20" priority="2">
+    <cfRule type="expression" dxfId="12" priority="6">
       <formula>AND(NOT(ISBLANK(E34)),OR(AND($D34="R",E34&lt;&gt;"V"),AND($D34="A",E34&lt;&gt;"M")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34:E38">
-    <cfRule type="expression" dxfId="19" priority="1">
+    <cfRule type="expression" dxfId="11" priority="5">
       <formula>AND(NOT(ISBLANK(E34)),OR(AND($D34="R",E34="V"),AND($D34="R",E34="v")))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F37">
+    <cfRule type="expression" dxfId="10" priority="4">
+      <formula>AND(NOT(ISBLANK(F2)),OR(AND($D2="R",F2&lt;&gt;"V"),AND($D2="A",F2&lt;&gt;"M")))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F37">
+    <cfRule type="expression" dxfId="9" priority="3">
+      <formula>AND(NOT(ISBLANK(F2)),OR(AND($D2="R",F2="V"),AND($D2="R",F2="v")))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2392,7 +2663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1C3D962-EA84-4A6E-9926-C561BC5A7D51}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
@@ -2900,22 +3171,22 @@
     <mergeCell ref="F1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="E2">
-    <cfRule type="expression" dxfId="10" priority="7">
+    <cfRule type="expression" dxfId="8" priority="7">
       <formula>AND(NOT(ISBLANK(E2)),OR(AND($D2="R",E2&lt;&gt;"V"),AND($D2="A",E2&lt;&gt;"M")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="7" priority="5">
       <formula>AND(NOT(ISBLANK(E2)),OR(AND($D2="R",E2="V"),AND($D2="R",E2="v")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E40">
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>AND(NOT(ISBLANK(E3)),OR(AND($D3="R",E3&lt;&gt;"V"),AND($D3="A",E3&lt;&gt;"M")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E40">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>AND(NOT(ISBLANK(E3)),OR(AND($D3="R",E3="V"),AND($D3="R",E3="v")))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2925,4 +3196,919 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E320CE66-A5E5-4BBD-BD32-8FE326D28843}">
+  <dimension ref="A1:J79"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D59" sqref="D59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="29.0625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.8125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1875" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.6875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.8125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="126.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A7" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A9" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A10" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A18" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A19" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A20" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A21" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A22" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A23" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A24" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A25" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A26" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A27" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A28" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A29" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A30" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A31" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A33" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A34" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A35" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A36" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A37" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A38" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A40" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A42" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A43" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A44" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A45" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A46" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A47" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A48" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A49" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A50" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A51" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A52" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A53" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A54" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A55" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D55" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A56" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D56" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A57" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D57" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A58" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A59" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D59" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A60" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A61" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D61" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A62" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A63" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A64" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A65" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D65" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A66" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D66" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A67" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D67" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A68" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A69" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D69" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A70" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A71" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A72" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D72" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A73" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D73" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A74" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A75" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D75" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A76" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D76" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A77" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D77" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A78" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D78" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A79" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G1:J1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F2:F37">
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>AND(NOT(ISBLANK(F2)),OR(AND($D2="R",F2&lt;&gt;"V"),AND($D2="A",F2&lt;&gt;"M")))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F37">
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>AND(NOT(ISBLANK(F2)),OR(AND($D2="R",F2="V"),AND($D2="R",F2="v")))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E37">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>AND(NOT(ISBLANK(E2)),OR(AND($D2="R",E2&lt;&gt;"V"),AND($D2="A",E2&lt;&gt;"M")))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E37">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>AND(NOT(ISBLANK(E2)),OR(AND($D2="R",E2="V"),AND($D2="R",E2="v")))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>